<commit_message>
Fix: adding ENUM type on Konten
</commit_message>
<xml_diff>
--- a/basdat_movie_data.xlsx
+++ b/basdat_movie_data.xlsx
@@ -39576,7 +39576,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>sutradara</t>
+          <t>type</t>
         </is>
       </c>
     </row>
@@ -39599,7 +39599,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -39620,7 +39624,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -39641,7 +39649,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -39662,7 +39674,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -39683,7 +39699,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -39704,7 +39724,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -39725,7 +39749,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -39746,7 +39774,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -39767,7 +39799,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -39788,7 +39824,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -39809,7 +39849,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -39830,7 +39874,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -39851,7 +39899,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -39872,7 +39924,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -39893,7 +39949,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -39914,7 +39974,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -39935,7 +39999,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -39956,7 +40024,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -39977,7 +40049,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -39998,7 +40074,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -40019,7 +40099,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -40040,7 +40124,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr"/>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -40061,7 +40149,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -40082,7 +40174,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -40103,7 +40199,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr"/>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -40124,7 +40224,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr"/>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -40145,7 +40249,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -40166,7 +40274,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr"/>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -40187,7 +40299,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr"/>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -40208,7 +40324,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr"/>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -40229,7 +40349,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr"/>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -40250,7 +40374,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr"/>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -40271,7 +40399,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr"/>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -40292,7 +40424,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr"/>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -40313,7 +40449,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr"/>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -40334,7 +40474,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr"/>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -40355,7 +40499,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr"/>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -40376,7 +40524,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr"/>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -40397,7 +40549,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr"/>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -40418,7 +40574,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr"/>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -40439,7 +40599,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr"/>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -40460,7 +40624,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr"/>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -40481,7 +40649,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr"/>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -40502,7 +40674,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr"/>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -40523,7 +40699,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr"/>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -40544,7 +40724,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr"/>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -40565,7 +40749,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr"/>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -40586,7 +40774,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr"/>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -40607,7 +40799,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr"/>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -40628,7 +40824,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr"/>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -40649,7 +40849,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr"/>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -40670,7 +40874,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr"/>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -40691,7 +40899,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr"/>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -40712,7 +40924,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr"/>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -40733,7 +40949,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr"/>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -40754,7 +40974,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr"/>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -40775,7 +40999,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr"/>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -40796,7 +41024,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr"/>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -40817,7 +41049,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr"/>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -40838,7 +41074,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr"/>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -40859,7 +41099,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr"/>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -40880,7 +41124,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr"/>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -40901,7 +41149,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr"/>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -40922,7 +41174,11 @@
           <t>SU</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr"/>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -40943,7 +41199,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr"/>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -40964,7 +41224,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr"/>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -40985,7 +41249,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr"/>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -41006,7 +41274,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr"/>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -41027,7 +41299,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr"/>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -41048,7 +41324,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr"/>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -41069,7 +41349,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr"/>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -41090,7 +41374,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr"/>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -41111,7 +41399,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr"/>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -41132,7 +41424,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr"/>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -41153,7 +41449,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr"/>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -41174,7 +41474,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E77" t="inlineStr"/>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -41195,7 +41499,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E78" t="inlineStr"/>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -41216,7 +41524,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr"/>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -41237,7 +41549,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E80" t="inlineStr"/>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -41258,7 +41574,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr"/>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -41279,7 +41599,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr"/>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -41300,7 +41624,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr"/>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -41321,7 +41649,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E84" t="inlineStr"/>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -41342,7 +41674,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E85" t="inlineStr"/>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -41363,7 +41699,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E86" t="inlineStr"/>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -41384,7 +41724,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E87" t="inlineStr"/>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -41405,7 +41749,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E88" t="inlineStr"/>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -41426,7 +41774,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E89" t="inlineStr"/>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -41447,7 +41799,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E90" t="inlineStr"/>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -41468,7 +41824,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E91" t="inlineStr"/>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -41489,7 +41849,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E92" t="inlineStr"/>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -41510,7 +41874,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E93" t="inlineStr"/>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -41531,7 +41899,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E94" t="inlineStr"/>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -41552,7 +41924,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E95" t="inlineStr"/>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -41573,7 +41949,11 @@
           <t>SU</t>
         </is>
       </c>
-      <c r="E96" t="inlineStr"/>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -41594,7 +41974,11 @@
           <t>SU</t>
         </is>
       </c>
-      <c r="E97" t="inlineStr"/>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -41615,7 +41999,11 @@
           <t>SU</t>
         </is>
       </c>
-      <c r="E98" t="inlineStr"/>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -41636,7 +42024,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E99" t="inlineStr"/>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -41657,7 +42049,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E100" t="inlineStr"/>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -41678,7 +42074,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E101" t="inlineStr"/>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -41699,7 +42099,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E102" t="inlineStr"/>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -41720,7 +42124,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E103" t="inlineStr"/>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -41741,7 +42149,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E104" t="inlineStr"/>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -41762,7 +42174,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E105" t="inlineStr"/>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -41783,7 +42199,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E106" t="inlineStr"/>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -41804,7 +42224,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E107" t="inlineStr"/>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -41825,7 +42249,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E108" t="inlineStr"/>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -41846,7 +42274,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E109" t="inlineStr"/>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -41867,7 +42299,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E110" t="inlineStr"/>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -41888,7 +42324,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E111" t="inlineStr"/>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -41909,7 +42349,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E112" t="inlineStr"/>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -41930,7 +42374,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E113" t="inlineStr"/>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -41951,7 +42399,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E114" t="inlineStr"/>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -41972,7 +42424,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E115" t="inlineStr"/>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -41993,7 +42449,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E116" t="inlineStr"/>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -42014,7 +42474,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E117" t="inlineStr"/>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -42035,7 +42499,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E118" t="inlineStr"/>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -42056,7 +42524,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E119" t="inlineStr"/>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -42077,7 +42549,11 @@
           <t>SU</t>
         </is>
       </c>
-      <c r="E120" t="inlineStr"/>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -42098,7 +42574,11 @@
           <t>SU</t>
         </is>
       </c>
-      <c r="E121" t="inlineStr"/>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -42119,7 +42599,11 @@
           <t>SU</t>
         </is>
       </c>
-      <c r="E122" t="inlineStr"/>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -42140,7 +42624,11 @@
           <t>SU</t>
         </is>
       </c>
-      <c r="E123" t="inlineStr"/>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -42161,7 +42649,11 @@
           <t>SU</t>
         </is>
       </c>
-      <c r="E124" t="inlineStr"/>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -42182,7 +42674,11 @@
           <t>SU</t>
         </is>
       </c>
-      <c r="E125" t="inlineStr"/>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -42203,7 +42699,11 @@
           <t>SU</t>
         </is>
       </c>
-      <c r="E126" t="inlineStr"/>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -42224,7 +42724,11 @@
           <t>SU</t>
         </is>
       </c>
-      <c r="E127" t="inlineStr"/>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -42245,7 +42749,11 @@
           <t>SU</t>
         </is>
       </c>
-      <c r="E128" t="inlineStr"/>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -42266,7 +42774,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E129" t="inlineStr"/>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -42287,7 +42799,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E130" t="inlineStr"/>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -42308,7 +42824,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E131" t="inlineStr"/>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -42329,7 +42849,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E132" t="inlineStr"/>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -42350,7 +42874,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E133" t="inlineStr"/>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -42371,7 +42899,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E134" t="inlineStr"/>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -42392,7 +42924,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E135" t="inlineStr"/>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -42413,7 +42949,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E136" t="inlineStr"/>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -42434,7 +42974,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E137" t="inlineStr"/>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -42455,7 +42999,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E138" t="inlineStr"/>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -42476,7 +43024,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E139" t="inlineStr"/>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -42497,7 +43049,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E140" t="inlineStr"/>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -42518,7 +43074,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E141" t="inlineStr"/>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -42539,7 +43099,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E142" t="inlineStr"/>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -42560,7 +43124,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E143" t="inlineStr"/>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -42581,7 +43149,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E144" t="inlineStr"/>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -42602,7 +43174,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E145" t="inlineStr"/>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -42623,7 +43199,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E146" t="inlineStr"/>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -42644,7 +43224,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E147" t="inlineStr"/>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -42665,7 +43249,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E148" t="inlineStr"/>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -42686,7 +43274,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E149" t="inlineStr"/>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -42707,7 +43299,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E150" t="inlineStr"/>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -42728,7 +43324,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E151" t="inlineStr"/>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -42749,7 +43349,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E152" t="inlineStr"/>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -42770,7 +43374,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E153" t="inlineStr"/>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -42791,7 +43399,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E154" t="inlineStr"/>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -42812,7 +43424,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E155" t="inlineStr"/>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -42833,7 +43449,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E156" t="inlineStr"/>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -42854,7 +43474,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E157" t="inlineStr"/>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -42875,7 +43499,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E158" t="inlineStr"/>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -42896,7 +43524,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E159" t="inlineStr"/>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -42917,7 +43549,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E160" t="inlineStr"/>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -42938,7 +43574,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E161" t="inlineStr"/>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -42959,7 +43599,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E162" t="inlineStr"/>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -42980,7 +43624,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E163" t="inlineStr"/>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -43001,7 +43649,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E164" t="inlineStr"/>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -43022,7 +43674,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E165" t="inlineStr"/>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -43043,7 +43699,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E166" t="inlineStr"/>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -43064,7 +43724,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E167" t="inlineStr"/>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -43085,7 +43749,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E168" t="inlineStr"/>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -43106,7 +43774,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E169" t="inlineStr"/>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -43127,7 +43799,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E170" t="inlineStr"/>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -43148,7 +43824,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E171" t="inlineStr"/>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -43169,7 +43849,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E172" t="inlineStr"/>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -43190,7 +43874,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E173" t="inlineStr"/>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -43211,7 +43899,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E174" t="inlineStr"/>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -43232,7 +43924,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E175" t="inlineStr"/>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -43253,7 +43949,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E176" t="inlineStr"/>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -43274,7 +43974,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E177" t="inlineStr"/>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -43295,7 +43999,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E178" t="inlineStr"/>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -43316,7 +44024,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E179" t="inlineStr"/>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -43337,7 +44049,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E180" t="inlineStr"/>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -43358,7 +44074,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E181" t="inlineStr"/>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -43379,7 +44099,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E182" t="inlineStr"/>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -43400,7 +44124,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E183" t="inlineStr"/>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -43421,7 +44149,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E184" t="inlineStr"/>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -43442,7 +44174,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E185" t="inlineStr"/>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -43463,7 +44199,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E186" t="inlineStr"/>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -43484,7 +44224,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E187" t="inlineStr"/>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -43505,7 +44249,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E188" t="inlineStr"/>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -43526,7 +44274,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E189" t="inlineStr"/>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -43547,7 +44299,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E190" t="inlineStr"/>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -43568,7 +44324,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E191" t="inlineStr"/>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -43589,7 +44349,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E192" t="inlineStr"/>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -43610,7 +44374,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E193" t="inlineStr"/>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -43631,7 +44399,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E194" t="inlineStr"/>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -43652,7 +44424,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E195" t="inlineStr"/>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -43673,7 +44449,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E196" t="inlineStr"/>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -43694,7 +44474,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E197" t="inlineStr"/>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -43715,7 +44499,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E198" t="inlineStr"/>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -43736,7 +44524,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E199" t="inlineStr"/>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -43757,7 +44549,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E200" t="inlineStr"/>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -43778,7 +44574,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E201" t="inlineStr"/>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -43799,7 +44599,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E202" t="inlineStr"/>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -43820,7 +44624,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E203" t="inlineStr"/>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -43841,7 +44649,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E204" t="inlineStr"/>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -43862,7 +44674,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E205" t="inlineStr"/>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -43883,7 +44699,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E206" t="inlineStr"/>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -43904,7 +44724,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E207" t="inlineStr"/>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -43925,7 +44749,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E208" t="inlineStr"/>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -43946,7 +44774,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E209" t="inlineStr"/>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -43967,7 +44799,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E210" t="inlineStr"/>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -43988,7 +44824,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E211" t="inlineStr"/>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -44009,7 +44849,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E212" t="inlineStr"/>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -44030,7 +44874,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E213" t="inlineStr"/>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -44051,7 +44899,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E214" t="inlineStr"/>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -44072,7 +44924,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E215" t="inlineStr"/>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -44093,7 +44949,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E216" t="inlineStr"/>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -44114,7 +44974,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E217" t="inlineStr"/>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -44135,7 +44999,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E218" t="inlineStr"/>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -44156,7 +45024,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E219" t="inlineStr"/>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -44177,7 +45049,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E220" t="inlineStr"/>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -44198,7 +45074,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E221" t="inlineStr"/>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -44219,7 +45099,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E222" t="inlineStr"/>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -44240,7 +45124,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E223" t="inlineStr"/>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -44261,7 +45149,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E224" t="inlineStr"/>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -44282,7 +45174,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E225" t="inlineStr"/>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -44303,7 +45199,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E226" t="inlineStr"/>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -44324,7 +45224,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E227" t="inlineStr"/>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -44345,7 +45249,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E228" t="inlineStr"/>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -44366,7 +45274,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E229" t="inlineStr"/>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -44387,7 +45299,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E230" t="inlineStr"/>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -44408,7 +45324,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E231" t="inlineStr"/>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -44429,7 +45349,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E232" t="inlineStr"/>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -44450,7 +45374,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E233" t="inlineStr"/>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -44471,7 +45399,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E234" t="inlineStr"/>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -44492,7 +45424,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E235" t="inlineStr"/>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -44513,7 +45449,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E236" t="inlineStr"/>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -44534,7 +45474,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E237" t="inlineStr"/>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -44555,7 +45499,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E238" t="inlineStr"/>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -44576,7 +45524,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E239" t="inlineStr"/>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -44597,7 +45549,11 @@
           <t>SU</t>
         </is>
       </c>
-      <c r="E240" t="inlineStr"/>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -44618,7 +45574,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E241" t="inlineStr"/>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -44639,7 +45599,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E242" t="inlineStr"/>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -44660,7 +45624,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E243" t="inlineStr"/>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -44681,7 +45649,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E244" t="inlineStr"/>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -44702,7 +45674,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E245" t="inlineStr"/>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -44723,7 +45699,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E246" t="inlineStr"/>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -44744,7 +45724,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E247" t="inlineStr"/>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -44765,7 +45749,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E248" t="inlineStr"/>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -44786,7 +45774,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E249" t="inlineStr"/>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -44807,7 +45799,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E250" t="inlineStr"/>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -44828,7 +45824,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E251" t="inlineStr"/>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -44849,7 +45849,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E252" t="inlineStr"/>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -44870,7 +45874,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E253" t="inlineStr"/>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -44891,7 +45899,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E254" t="inlineStr"/>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -44912,7 +45924,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E255" t="inlineStr"/>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -44933,7 +45949,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E256" t="inlineStr"/>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -44954,7 +45974,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E257" t="inlineStr"/>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -44975,7 +45999,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E258" t="inlineStr"/>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -44996,7 +46024,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E259" t="inlineStr"/>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -45017,7 +46049,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E260" t="inlineStr"/>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -45038,7 +46074,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E261" t="inlineStr"/>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -45059,7 +46099,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E262" t="inlineStr"/>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -45080,7 +46124,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E263" t="inlineStr"/>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -45101,7 +46149,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E264" t="inlineStr"/>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -45122,7 +46174,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E265" t="inlineStr"/>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -45143,7 +46199,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E266" t="inlineStr"/>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -45164,7 +46224,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E267" t="inlineStr"/>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -45185,7 +46249,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E268" t="inlineStr"/>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -45206,7 +46274,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E269" t="inlineStr"/>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -45227,7 +46299,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E270" t="inlineStr"/>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -45248,7 +46324,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E271" t="inlineStr"/>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -45269,7 +46349,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E272" t="inlineStr"/>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -45290,7 +46374,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E273" t="inlineStr"/>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -45311,7 +46399,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E274" t="inlineStr"/>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -45332,7 +46424,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E275" t="inlineStr"/>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -45353,7 +46449,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E276" t="inlineStr"/>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -45374,7 +46474,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E277" t="inlineStr"/>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -45395,7 +46499,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E278" t="inlineStr"/>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -45416,7 +46524,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E279" t="inlineStr"/>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -45437,7 +46549,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E280" t="inlineStr"/>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -45458,7 +46574,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E281" t="inlineStr"/>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -45479,7 +46599,11 @@
           <t>17+</t>
         </is>
       </c>
-      <c r="E282" t="inlineStr"/>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -45500,7 +46624,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E283" t="inlineStr"/>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -45521,7 +46649,11 @@
           <t>13+</t>
         </is>
       </c>
-      <c r="E284" t="inlineStr"/>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -45542,7 +46674,11 @@
           <t>TV-Y7</t>
         </is>
       </c>
-      <c r="E285" t="inlineStr"/>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -45563,7 +46699,11 @@
           <t>TV-MA</t>
         </is>
       </c>
-      <c r="E286" t="inlineStr"/>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -45584,7 +46724,11 @@
           <t>TV-14</t>
         </is>
       </c>
-      <c r="E287" t="inlineStr"/>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>Serial_TV</t>
+        </is>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -45607,7 +46751,7 @@
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>Christopher Nolan</t>
+          <t>Film</t>
         </is>
       </c>
     </row>
@@ -45632,7 +46776,7 @@
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>Christopher Nolan</t>
+          <t>Film</t>
         </is>
       </c>
     </row>
@@ -45657,7 +46801,7 @@
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>Bong Joon Ho</t>
+          <t>Film</t>
         </is>
       </c>
     </row>
@@ -45680,7 +46824,11 @@
           <t>R</t>
         </is>
       </c>
-      <c r="E291" t="inlineStr"/>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -45701,7 +46849,11 @@
           <t>PG-13</t>
         </is>
       </c>
-      <c r="E292" t="inlineStr"/>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -45722,7 +46874,11 @@
           <t>PG-13</t>
         </is>
       </c>
-      <c r="E293" t="inlineStr"/>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -45743,7 +46899,11 @@
           <t>PG</t>
         </is>
       </c>
-      <c r="E294" t="inlineStr"/>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -45764,7 +46924,11 @@
           <t>PG-13</t>
         </is>
       </c>
-      <c r="E295" t="inlineStr"/>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -45785,7 +46949,11 @@
           <t>PG-13</t>
         </is>
       </c>
-      <c r="E296" t="inlineStr"/>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -45806,7 +46974,11 @@
           <t>PG-13</t>
         </is>
       </c>
-      <c r="E297" t="inlineStr"/>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -45827,7 +46999,11 @@
           <t>PG-13</t>
         </is>
       </c>
-      <c r="E298" t="inlineStr"/>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -45848,7 +47024,11 @@
           <t>PG-13</t>
         </is>
       </c>
-      <c r="E299" t="inlineStr"/>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -45869,7 +47049,11 @@
           <t>R</t>
         </is>
       </c>
-      <c r="E300" t="inlineStr"/>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -45890,7 +47074,11 @@
           <t>R</t>
         </is>
       </c>
-      <c r="E301" t="inlineStr"/>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -45911,7 +47099,11 @@
           <t>R</t>
         </is>
       </c>
-      <c r="E302" t="inlineStr"/>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -45932,7 +47124,11 @@
           <t>PG-13</t>
         </is>
       </c>
-      <c r="E303" t="inlineStr"/>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -45953,7 +47149,11 @@
           <t>R</t>
         </is>
       </c>
-      <c r="E304" t="inlineStr"/>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -45974,7 +47174,11 @@
           <t>R</t>
         </is>
       </c>
-      <c r="E305" t="inlineStr"/>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -45995,7 +47199,11 @@
           <t>PG-13</t>
         </is>
       </c>
-      <c r="E306" t="inlineStr"/>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -46016,7 +47224,11 @@
           <t>PG-13</t>
         </is>
       </c>
-      <c r="E307" t="inlineStr"/>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -46037,7 +47249,11 @@
           <t>R</t>
         </is>
       </c>
-      <c r="E308" t="inlineStr"/>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
@@ -46058,7 +47274,11 @@
           <t>PG-13</t>
         </is>
       </c>
-      <c r="E309" t="inlineStr"/>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
@@ -46079,7 +47299,11 @@
           <t>R</t>
         </is>
       </c>
-      <c r="E310" t="inlineStr"/>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update Peran roles and exports
</commit_message>
<xml_diff>
--- a/basdat_movie_data.xlsx
+++ b/basdat_movie_data.xlsx
@@ -7170,7 +7170,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Tony Stark</t>
         </is>
       </c>
     </row>
@@ -7187,7 +7187,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Tony Stark</t>
         </is>
       </c>
     </row>
@@ -7204,7 +7204,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Tony Stark</t>
         </is>
       </c>
     </row>
@@ -7221,7 +7221,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Tony Stark</t>
         </is>
       </c>
     </row>
@@ -7238,7 +7238,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Steve Rogers</t>
         </is>
       </c>
     </row>
@@ -7255,7 +7255,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Thor</t>
         </is>
       </c>
     </row>
@@ -7272,7 +7272,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Bruce Banner</t>
         </is>
       </c>
     </row>
@@ -7289,7 +7289,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Thor</t>
         </is>
       </c>
     </row>
@@ -7306,7 +7306,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Thor</t>
         </is>
       </c>
     </row>
@@ -7323,7 +7323,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Thor</t>
         </is>
       </c>
     </row>
@@ -7340,7 +7340,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Steve Rogers</t>
         </is>
       </c>
     </row>
@@ -7357,7 +7357,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Steve Rogers</t>
         </is>
       </c>
     </row>
@@ -7374,7 +7374,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Steve Rogers</t>
         </is>
       </c>
     </row>
@@ -7391,7 +7391,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>T'Challa</t>
         </is>
       </c>
     </row>
@@ -7408,7 +7408,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Stephen Strange</t>
         </is>
       </c>
     </row>
@@ -7425,7 +7425,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Stephen Strange</t>
         </is>
       </c>
     </row>
@@ -7442,7 +7442,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Peter Parker</t>
         </is>
       </c>
     </row>
@@ -7459,7 +7459,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Peter Parker</t>
         </is>
       </c>
     </row>
@@ -7476,7 +7476,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Peter Parker</t>
         </is>
       </c>
     </row>
@@ -7493,7 +7493,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Scott Lang</t>
         </is>
       </c>
     </row>
@@ -7510,7 +7510,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Scott Lang</t>
         </is>
       </c>
     </row>
@@ -7527,7 +7527,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Natasha Romanoff</t>
         </is>
       </c>
     </row>
@@ -7544,7 +7544,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Xu Shang-Chi</t>
         </is>
       </c>
     </row>
@@ -7561,7 +7561,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Sersi</t>
         </is>
       </c>
     </row>
@@ -7578,7 +7578,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Dom Cobb</t>
         </is>
       </c>
     </row>
@@ -7595,7 +7595,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Bruce Wayne</t>
         </is>
       </c>
     </row>
@@ -7612,7 +7612,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Bruce Wayne</t>
         </is>
       </c>
     </row>
@@ -7629,7 +7629,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Bruce Wayne</t>
         </is>
       </c>
     </row>
@@ -7646,7 +7646,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Cooper</t>
         </is>
       </c>
     </row>
@@ -7663,7 +7663,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Tommy</t>
         </is>
       </c>
     </row>
@@ -7680,7 +7680,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>The Protagonist</t>
         </is>
       </c>
     </row>
@@ -7697,7 +7697,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>J. Robert Oppenheimer</t>
         </is>
       </c>
     </row>
@@ -7714,7 +7714,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Arthur Fleck</t>
         </is>
       </c>
     </row>
@@ -7731,7 +7731,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jack Dawson</t>
         </is>
       </c>
     </row>
@@ -7748,7 +7748,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jake Sully</t>
         </is>
       </c>
     </row>
@@ -7765,7 +7765,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jake Sully</t>
         </is>
       </c>
     </row>
@@ -7782,7 +7782,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Neo</t>
         </is>
       </c>
     </row>
@@ -7799,7 +7799,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Neo</t>
         </is>
       </c>
     </row>
@@ -7816,7 +7816,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Neo</t>
         </is>
       </c>
     </row>
@@ -7833,7 +7833,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>John Wick</t>
         </is>
       </c>
     </row>
@@ -7850,7 +7850,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>John Wick</t>
         </is>
       </c>
     </row>
@@ -7867,7 +7867,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>John Wick</t>
         </is>
       </c>
     </row>
@@ -7884,7 +7884,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>John Wick</t>
         </is>
       </c>
     </row>
@@ -7901,7 +7901,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Ethan Hunt</t>
         </is>
       </c>
     </row>
@@ -7918,7 +7918,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Ethan Hunt</t>
         </is>
       </c>
     </row>
@@ -7935,7 +7935,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Pete "Maverick" Mitchell</t>
         </is>
       </c>
     </row>
@@ -7952,7 +7952,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Pete "Maverick" Mitchell</t>
         </is>
       </c>
     </row>
@@ -7969,7 +7969,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Maximus Decimus Meridius</t>
         </is>
       </c>
     </row>
@@ -7986,7 +7986,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Michael Corleone</t>
         </is>
       </c>
     </row>
@@ -8003,7 +8003,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Michael Corleone</t>
         </is>
       </c>
     </row>
@@ -8020,7 +8020,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Vincent Vega</t>
         </is>
       </c>
     </row>
@@ -8037,7 +8037,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Tyler Durden</t>
         </is>
       </c>
     </row>
@@ -8054,7 +8054,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Forrest Gump</t>
         </is>
       </c>
     </row>
@@ -8071,7 +8071,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Andy Dufresne</t>
         </is>
       </c>
     </row>
@@ -8088,7 +8088,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Kim Ki-taek</t>
         </is>
       </c>
     </row>
@@ -8105,7 +8105,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Seok-woo</t>
         </is>
       </c>
     </row>
@@ -8122,7 +8122,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Rama</t>
         </is>
       </c>
     </row>
@@ -8139,7 +8139,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Rama</t>
         </is>
       </c>
     </row>
@@ -8156,7 +8156,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Sancaka</t>
         </is>
       </c>
     </row>
@@ -8173,7 +8173,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Alana</t>
         </is>
       </c>
     </row>
@@ -8190,7 +8190,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Rini</t>
         </is>
       </c>
     </row>
@@ -8207,7 +8207,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Rini</t>
         </is>
       </c>
     </row>
@@ -8224,7 +8224,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Nur</t>
         </is>
       </c>
     </row>
@@ -8241,7 +8241,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Bu Muslimah</t>
         </is>
       </c>
     </row>
@@ -8258,7 +8258,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>B. J. Habibie</t>
         </is>
       </c>
     </row>
@@ -8275,7 +8275,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Dilan</t>
         </is>
       </c>
     </row>
@@ -8292,7 +8292,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Dilan</t>
         </is>
       </c>
     </row>
@@ -8309,7 +8309,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Dilan</t>
         </is>
       </c>
     </row>
@@ -8326,7 +8326,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Cinta</t>
         </is>
       </c>
     </row>
@@ -8343,7 +8343,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Cinta</t>
         </is>
       </c>
     </row>
@@ -8360,7 +8360,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Erwin</t>
         </is>
       </c>
     </row>
@@ -8377,7 +8377,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Pak Domu</t>
         </is>
       </c>
     </row>
@@ -8394,7 +8394,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Piko</t>
         </is>
       </c>
     </row>
@@ -8411,7 +8411,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Topan</t>
         </is>
       </c>
     </row>
@@ -8428,7 +8428,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Maya</t>
         </is>
       </c>
     </row>
@@ -8445,7 +8445,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Adrian</t>
         </is>
       </c>
     </row>
@@ -8462,7 +8462,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Alfie</t>
         </is>
       </c>
     </row>
@@ -8479,7 +8479,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Hanif</t>
         </is>
       </c>
     </row>
@@ -8496,7 +8496,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Suzzanna</t>
         </is>
       </c>
     </row>
@@ -8513,7 +8513,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>The Girl</t>
         </is>
       </c>
     </row>
@@ -8530,7 +8530,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Oh Dae-su</t>
         </is>
       </c>
     </row>
@@ -8547,7 +8547,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Park Doo-man</t>
         </is>
       </c>
     </row>
@@ -8564,7 +8564,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jacob Yi</t>
         </is>
       </c>
     </row>
@@ -8581,7 +8581,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Song Seo-rae</t>
         </is>
       </c>
     </row>
@@ -8598,7 +8598,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Sang-hyun</t>
         </is>
       </c>
     </row>
@@ -8615,7 +8615,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Lee Jong-su</t>
         </is>
       </c>
     </row>
@@ -8632,7 +8632,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Chief Go</t>
         </is>
       </c>
     </row>
@@ -8649,7 +8649,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Yong-nam</t>
         </is>
       </c>
     </row>
@@ -8666,7 +8666,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Kim Ja-hong</t>
         </is>
       </c>
     </row>
@@ -8683,7 +8683,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Gang-lim</t>
         </is>
       </c>
     </row>
@@ -8700,7 +8700,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jong-goo</t>
         </is>
       </c>
     </row>
@@ -8717,7 +8717,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Kim Soo-hyun</t>
         </is>
       </c>
     </row>
@@ -8734,7 +8734,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Kim Man-seob</t>
         </is>
       </c>
     </row>
@@ -8751,7 +8751,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Lee Yong-gu</t>
         </is>
       </c>
     </row>
@@ -8768,7 +8768,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Harry Potter</t>
         </is>
       </c>
     </row>
@@ -8785,7 +8785,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Harry Potter</t>
         </is>
       </c>
     </row>
@@ -8802,7 +8802,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Harry Potter</t>
         </is>
       </c>
     </row>
@@ -8819,7 +8819,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Harry Potter</t>
         </is>
       </c>
     </row>
@@ -8836,7 +8836,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Harry Potter</t>
         </is>
       </c>
     </row>
@@ -8853,7 +8853,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Harry Potter</t>
         </is>
       </c>
     </row>
@@ -8870,7 +8870,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Harry Potter</t>
         </is>
       </c>
     </row>
@@ -8887,7 +8887,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Harry Potter</t>
         </is>
       </c>
     </row>
@@ -8904,7 +8904,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Newt Scamander</t>
         </is>
       </c>
     </row>
@@ -8921,7 +8921,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Newt Scamander</t>
         </is>
       </c>
     </row>
@@ -8938,7 +8938,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Newt Scamander</t>
         </is>
       </c>
     </row>
@@ -8955,7 +8955,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Frodo Baggins</t>
         </is>
       </c>
     </row>
@@ -8972,7 +8972,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Frodo Baggins</t>
         </is>
       </c>
     </row>
@@ -8989,7 +8989,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Frodo Baggins</t>
         </is>
       </c>
     </row>
@@ -9006,7 +9006,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Bilbo Baggins</t>
         </is>
       </c>
     </row>
@@ -9023,7 +9023,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Bilbo Baggins</t>
         </is>
       </c>
     </row>
@@ -9040,7 +9040,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Bilbo Baggins</t>
         </is>
       </c>
     </row>
@@ -9057,7 +9057,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jack Sparrow</t>
         </is>
       </c>
     </row>
@@ -9074,7 +9074,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jack Sparrow</t>
         </is>
       </c>
     </row>
@@ -9091,7 +9091,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jack Sparrow</t>
         </is>
       </c>
     </row>
@@ -9108,7 +9108,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Alan Grant</t>
         </is>
       </c>
     </row>
@@ -9125,7 +9125,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Owen Grady</t>
         </is>
       </c>
     </row>
@@ -9142,7 +9142,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Owen Grady</t>
         </is>
       </c>
     </row>
@@ -9159,7 +9159,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Martin Brody</t>
         </is>
       </c>
     </row>
@@ -9176,7 +9176,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Elliott</t>
         </is>
       </c>
     </row>
@@ -9193,7 +9193,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Marty McFly</t>
         </is>
       </c>
     </row>
@@ -9210,7 +9210,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Marty McFly</t>
         </is>
       </c>
     </row>
@@ -9227,7 +9227,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Marty McFly</t>
         </is>
       </c>
     </row>
@@ -9244,7 +9244,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Luke Skywalker</t>
         </is>
       </c>
     </row>
@@ -9261,7 +9261,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Luke Skywalker</t>
         </is>
       </c>
     </row>
@@ -9278,7 +9278,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Luke Skywalker</t>
         </is>
       </c>
     </row>
@@ -9295,7 +9295,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Obi-Wan Kenobi</t>
         </is>
       </c>
     </row>
@@ -9312,7 +9312,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Anakin Skywalker</t>
         </is>
       </c>
     </row>
@@ -9329,7 +9329,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Anakin Skywalker</t>
         </is>
       </c>
     </row>
@@ -9346,7 +9346,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Carol Danvers</t>
         </is>
       </c>
     </row>
@@ -9363,7 +9363,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Peter Quill</t>
         </is>
       </c>
     </row>
@@ -9380,7 +9380,7 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Peter Quill</t>
         </is>
       </c>
     </row>
@@ -9397,7 +9397,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Peter Quill</t>
         </is>
       </c>
     </row>
@@ -9414,7 +9414,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Shuri</t>
         </is>
       </c>
     </row>
@@ -9431,7 +9431,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Maruo Ichinose</t>
         </is>
       </c>
     </row>
@@ -9448,7 +9448,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Loki</t>
         </is>
       </c>
     </row>
@@ -9465,7 +9465,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Wanda Maximoff</t>
         </is>
       </c>
     </row>
@@ -9482,7 +9482,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Clint Barton</t>
         </is>
       </c>
     </row>
@@ -9499,7 +9499,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Marc Spector</t>
         </is>
       </c>
     </row>
@@ -9516,7 +9516,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jennifer Walters</t>
         </is>
       </c>
     </row>
@@ -9533,7 +9533,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Sam Wilson</t>
         </is>
       </c>
     </row>
@@ -9550,7 +9550,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Matt Murdock</t>
         </is>
       </c>
     </row>
@@ -9567,7 +9567,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jessica Jones</t>
         </is>
       </c>
     </row>
@@ -9584,7 +9584,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Frank Castle</t>
         </is>
       </c>
     </row>
@@ -9601,7 +9601,7 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Phil Coulson</t>
         </is>
       </c>
     </row>
@@ -9618,7 +9618,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Luke Cage</t>
         </is>
       </c>
     </row>
@@ -9635,7 +9635,7 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Danny Rand</t>
         </is>
       </c>
     </row>
@@ -9652,7 +9652,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Nick Fury</t>
         </is>
       </c>
     </row>
@@ -9669,7 +9669,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Grandmaster</t>
         </is>
       </c>
     </row>
@@ -9686,7 +9686,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Walter White</t>
         </is>
       </c>
     </row>
@@ -9703,7 +9703,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jimmy McGill</t>
         </is>
       </c>
     </row>
@@ -9720,7 +9720,7 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Daenerys Targaryen</t>
         </is>
       </c>
     </row>
@@ -9737,7 +9737,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Rhaenyra Targaryen</t>
         </is>
       </c>
     </row>
@@ -9754,7 +9754,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Eleven</t>
         </is>
       </c>
     </row>
@@ -9771,7 +9771,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Geralt of Rivia</t>
         </is>
       </c>
     </row>
@@ -9788,7 +9788,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Din Djarin</t>
         </is>
       </c>
     </row>
@@ -9805,7 +9805,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Joel Miller</t>
         </is>
       </c>
     </row>
@@ -9822,7 +9822,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Thomas Shelby</t>
         </is>
       </c>
     </row>
@@ -9839,7 +9839,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Sherlock Holmes</t>
         </is>
       </c>
     </row>
@@ -9856,7 +9856,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Dexter Morgan</t>
         </is>
       </c>
     </row>
@@ -9873,7 +9873,7 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Carrie Mathison</t>
         </is>
       </c>
     </row>
@@ -9890,7 +9890,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Dolores Abernathy</t>
         </is>
       </c>
     </row>
@@ -9907,7 +9907,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Rust Cohle</t>
         </is>
       </c>
     </row>
@@ -9924,7 +9924,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Billy Butcher</t>
         </is>
       </c>
     </row>
@@ -9941,7 +9941,7 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Mark Grayson</t>
         </is>
       </c>
     </row>
@@ -9958,7 +9958,7 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Viktor Hargreeves</t>
         </is>
       </c>
     </row>
@@ -9975,7 +9975,7 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Pablo Escobar</t>
         </is>
       </c>
     </row>
@@ -9992,7 +9992,7 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>The Professor</t>
         </is>
       </c>
     </row>
@@ -10009,7 +10009,7 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jonas Kahnwald</t>
         </is>
       </c>
     </row>
@@ -10026,7 +10026,7 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Valery Legasov</t>
         </is>
       </c>
     </row>
@@ -10043,7 +10043,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Cliff Stanfield</t>
         </is>
       </c>
     </row>
@@ -10060,7 +10060,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Lester Nygaard</t>
         </is>
       </c>
     </row>
@@ -10077,7 +10077,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jack Shephard</t>
         </is>
       </c>
     </row>
@@ -10094,7 +10094,7 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Michael Scofield</t>
         </is>
       </c>
     </row>
@@ -10111,7 +10111,7 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jack Bauer</t>
         </is>
       </c>
     </row>
@@ -10128,7 +10128,7 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Michael Scott</t>
         </is>
       </c>
     </row>
@@ -10145,7 +10145,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Rachel Green</t>
         </is>
       </c>
     </row>
@@ -10162,7 +10162,7 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Ted Mosby</t>
         </is>
       </c>
     </row>
@@ -10179,7 +10179,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jerry Seinfeld</t>
         </is>
       </c>
     </row>
@@ -10196,7 +10196,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jay Pritchett</t>
         </is>
       </c>
     </row>
@@ -10213,7 +10213,7 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jake Peralta</t>
         </is>
       </c>
     </row>
@@ -10230,7 +10230,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Leslie Knope</t>
         </is>
       </c>
     </row>
@@ -10247,7 +10247,7 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Harvey Specter</t>
         </is>
       </c>
     </row>
@@ -10264,7 +10264,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Gregory House</t>
         </is>
       </c>
     </row>
@@ -10281,7 +10281,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Meredith Grey</t>
         </is>
       </c>
     </row>
@@ -10298,7 +10298,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Gil Grissom</t>
         </is>
       </c>
     </row>
@@ -10315,7 +10315,7 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Leroy Jethro Gibbs</t>
         </is>
       </c>
     </row>
@@ -10332,7 +10332,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jason Gideon</t>
         </is>
       </c>
     </row>
@@ -10349,7 +10349,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Olivia Benson</t>
         </is>
       </c>
     </row>
@@ -10366,7 +10366,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Dean Winchester</t>
         </is>
       </c>
     </row>
@@ -10383,7 +10383,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Clark Kent</t>
         </is>
       </c>
     </row>
@@ -10400,7 +10400,7 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Oliver Queen</t>
         </is>
       </c>
     </row>
@@ -10417,7 +10417,7 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Barry Allen</t>
         </is>
       </c>
     </row>
@@ -10434,7 +10434,7 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Sara Lance</t>
         </is>
       </c>
     </row>
@@ -10451,7 +10451,7 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jim Gordon</t>
         </is>
       </c>
     </row>
@@ -10468,7 +10468,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Dick Grayson</t>
         </is>
       </c>
     </row>
@@ -10485,7 +10485,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Cliff Steele</t>
         </is>
       </c>
     </row>
@@ -10502,7 +10502,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>James Holden</t>
         </is>
       </c>
     </row>
@@ -10519,7 +10519,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>William Adama</t>
         </is>
       </c>
     </row>
@@ -10536,7 +10536,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Malcolm Reynolds</t>
         </is>
       </c>
     </row>
@@ -10553,7 +10553,7 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Olivia Dunham</t>
         </is>
       </c>
     </row>
@@ -10570,7 +10570,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Rick Grimes</t>
         </is>
       </c>
     </row>
@@ -10587,7 +10587,7 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Madison Clark</t>
         </is>
       </c>
     </row>
@@ -10604,7 +10604,7 @@
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Hannibal Lecter</t>
         </is>
       </c>
     </row>
@@ -10621,7 +10621,7 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Ragnar Lothbrok</t>
         </is>
       </c>
     </row>
@@ -10638,7 +10638,7 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Leif Erikson</t>
         </is>
       </c>
     </row>
@@ -10655,7 +10655,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Captain Flint</t>
         </is>
       </c>
     </row>
@@ -10672,7 +10672,7 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Lucius Vorenus</t>
         </is>
       </c>
     </row>
@@ -10689,7 +10689,7 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Spartacus</t>
         </is>
       </c>
     </row>
@@ -10706,7 +10706,7 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Scott McCall</t>
         </is>
       </c>
     </row>
@@ -10723,7 +10723,7 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Archie Andrews</t>
         </is>
       </c>
     </row>
@@ -10740,7 +10740,7 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Lucifer Morningstar</t>
         </is>
       </c>
     </row>
@@ -10757,7 +10757,7 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Sun Bak</t>
         </is>
       </c>
     </row>
@@ -10774,7 +10774,7 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Elliot Alderson</t>
         </is>
       </c>
     </row>
@@ -10791,7 +10791,7 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Queen Elizabeth II</t>
         </is>
       </c>
     </row>
@@ -10808,7 +10808,7 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>June Osborne</t>
         </is>
       </c>
     </row>
@@ -10825,7 +10825,7 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>John Dutton</t>
         </is>
       </c>
     </row>
@@ -10842,7 +10842,7 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Marty Byrde</t>
         </is>
       </c>
     </row>
@@ -10859,7 +10859,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Don Draper</t>
         </is>
       </c>
     </row>
@@ -10876,7 +10876,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Nucky Thompson</t>
         </is>
       </c>
     </row>
@@ -10893,7 +10893,7 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Mare Sheehan</t>
         </is>
       </c>
     </row>
@@ -10910,7 +10910,7 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Logan Roy</t>
         </is>
       </c>
     </row>
@@ -10927,7 +10927,7 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Mark Scout</t>
         </is>
       </c>
     </row>
@@ -10944,7 +10944,7 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Cassian Andor</t>
         </is>
       </c>
     </row>
@@ -10961,7 +10961,7 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Obi-Wan Kenobi</t>
         </is>
       </c>
     </row>
@@ -10978,7 +10978,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Ahsoka Tano</t>
         </is>
       </c>
     </row>
@@ -10995,7 +10995,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Michael Burnham</t>
         </is>
       </c>
     </row>
@@ -11012,7 +11012,7 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jean-Luc Picard</t>
         </is>
       </c>
     </row>
@@ -11029,7 +11029,7 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Shaun Murphy</t>
         </is>
       </c>
     </row>
@@ -11046,7 +11046,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jack Pearson</t>
         </is>
       </c>
     </row>
@@ -11063,7 +11063,7 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Patrick Jane</t>
         </is>
       </c>
     </row>
@@ -11080,7 +11080,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>John Reese</t>
         </is>
       </c>
     </row>
@@ -11097,7 +11097,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Sherlock Holmes</t>
         </is>
       </c>
     </row>
@@ -11114,7 +11114,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Lyra Silvertongue</t>
         </is>
       </c>
     </row>
@@ -11131,7 +11131,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Morpheus</t>
         </is>
       </c>
     </row>
@@ -11148,7 +11148,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Snow</t>
         </is>
       </c>
     </row>
@@ -11165,7 +11165,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Vi</t>
         </is>
       </c>
     </row>
@@ -11182,7 +11182,7 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Trevor Belmont</t>
         </is>
       </c>
     </row>
@@ -11199,7 +11199,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Callum</t>
         </is>
       </c>
     </row>
@@ -11216,7 +11216,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Aang</t>
         </is>
       </c>
     </row>
@@ -11233,7 +11233,7 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Korra</t>
         </is>
       </c>
     </row>
@@ -11250,7 +11250,7 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Seong Gi-hun</t>
         </is>
       </c>
     </row>
@@ -11267,7 +11267,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Lee Chang</t>
         </is>
       </c>
     </row>
@@ -11284,7 +11284,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Ri Jeong-hyeok</t>
         </is>
       </c>
     </row>
@@ -11301,7 +11301,7 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Kim Shin</t>
         </is>
       </c>
     </row>
@@ -11318,7 +11318,7 @@
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Yoo Si-jin</t>
         </is>
       </c>
     </row>
@@ -11335,7 +11335,7 @@
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Park Sae-ro-yi</t>
         </is>
       </c>
     </row>
@@ -11352,7 +11352,7 @@
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Vincenzo Cassano</t>
         </is>
       </c>
     </row>
@@ -11369,7 +11369,7 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Choi Taek</t>
         </is>
       </c>
     </row>
@@ -11386,7 +11386,7 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Park Hae-young</t>
         </is>
       </c>
     </row>
@@ -11403,7 +11403,7 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Lee Ik-jun</t>
         </is>
       </c>
     </row>
@@ -11420,7 +11420,7 @@
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Park Dong-hoon</t>
         </is>
       </c>
     </row>
@@ -11437,7 +11437,7 @@
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Nam On-jo</t>
         </is>
       </c>
     </row>
@@ -11454,7 +11454,7 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Cha Hyun-soo</t>
         </is>
       </c>
     </row>
@@ -11471,7 +11471,7 @@
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Woo Young-woo</t>
         </is>
       </c>
     </row>
@@ -11488,7 +11488,7 @@
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Jung Jin-soo</t>
         </is>
       </c>
     </row>
@@ -11505,7 +11505,7 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Eren Yeager</t>
         </is>
       </c>
     </row>
@@ -11522,7 +11522,7 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Naruto Uzumaki</t>
         </is>
       </c>
     </row>
@@ -11539,7 +11539,7 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Naruto Uzumaki</t>
         </is>
       </c>
     </row>
@@ -11556,7 +11556,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Ichigo Kurosaki</t>
         </is>
       </c>
     </row>
@@ -11573,7 +11573,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Monkey D. Luffy</t>
         </is>
       </c>
     </row>
@@ -11590,7 +11590,7 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Tanjiro Kamado</t>
         </is>
       </c>
     </row>
@@ -11607,7 +11607,7 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Yuji Itadori</t>
         </is>
       </c>
     </row>
@@ -11624,7 +11624,7 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Izuku Midoriya</t>
         </is>
       </c>
     </row>
@@ -11641,7 +11641,7 @@
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Edward Elric</t>
         </is>
       </c>
     </row>
@@ -11658,7 +11658,7 @@
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Light Yagami</t>
         </is>
       </c>
     </row>
@@ -11675,7 +11675,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Gon Freecss</t>
         </is>
       </c>
     </row>
@@ -11692,7 +11692,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Denji</t>
         </is>
       </c>
     </row>
@@ -11709,7 +11709,7 @@
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Ken Kaneki</t>
         </is>
       </c>
     </row>
@@ -11726,7 +11726,7 @@
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Kirito</t>
         </is>
       </c>
     </row>
@@ -11743,7 +11743,7 @@
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Asta</t>
         </is>
       </c>
     </row>
@@ -11760,7 +11760,7 @@
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Natsu Dragneel</t>
         </is>
       </c>
     </row>
@@ -11777,7 +11777,7 @@
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Shoyo Hinata</t>
         </is>
       </c>
     </row>
@@ -11794,7 +11794,7 @@
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Yoichi Isagi</t>
         </is>
       </c>
     </row>
@@ -11811,7 +11811,7 @@
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Loid Forger</t>
         </is>
       </c>
     </row>
@@ -11828,7 +11828,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Senku Ishigami</t>
         </is>
       </c>
     </row>
@@ -11845,7 +11845,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Shigeo Kageyama</t>
         </is>
       </c>
     </row>
@@ -11862,7 +11862,7 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Thorfinn</t>
         </is>
       </c>
     </row>
@@ -11879,7 +11879,7 @@
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Aris</t>
         </is>
       </c>
     </row>
@@ -11896,7 +11896,7 @@
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Dasiyah</t>
         </is>
       </c>
     </row>
@@ -11913,7 +11913,7 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Suci</t>
         </is>
       </c>
     </row>
@@ -11930,7 +11930,7 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Andreas</t>
         </is>
       </c>
     </row>
@@ -11947,7 +11947,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Bian</t>
         </is>
       </c>
     </row>
@@ -11964,7 +11964,7 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>Talita</t>
         </is>
       </c>
     </row>

</xml_diff>